<commit_message>
add processin option for dissolving lakes
</commit_message>
<xml_diff>
--- a/tdxhydrorapid/network_data/processing_options.xlsx
+++ b/tdxhydrorapid/network_data/processing_options.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rchales/code/tdxhydro-postprocessing/tdxhydrorapid/network_data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ricky/tdxhydro-postprocessing/tdxhydrorapid/network_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4259F540-F3FE-B449-9C02-C252E5DDE208}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23A23C73-A551-C147-82F6-B1ECE8D77723}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20" yWindow="500" windowWidth="34560" windowHeight="20120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>min_stream_order</t>
   </si>
@@ -56,6 +56,9 @@
   </si>
   <si>
     <t>stream_count</t>
+  </si>
+  <si>
+    <t>dissolve_lakes</t>
   </si>
 </sst>
 </file>
@@ -551,11 +554,10 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -615,9 +617,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -655,7 +657,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -761,7 +763,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -903,7 +905,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -911,11 +913,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K63"/>
+  <dimension ref="A1:L63"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A15" sqref="A15"/>
+      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N57" sqref="N57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -931,10 +933,9 @@
     <col min="9" max="9" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="17.1640625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="19.5" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -968,8 +969,11 @@
       <c r="K1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1020000010</v>
       </c>
@@ -1003,8 +1007,11 @@
       <c r="K2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1020011530</v>
       </c>
@@ -1038,8 +1045,11 @@
       <c r="K3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1020018110</v>
       </c>
@@ -1073,8 +1083,11 @@
       <c r="K4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1020021940</v>
       </c>
@@ -1108,8 +1121,11 @@
       <c r="K5">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>1020027430</v>
       </c>
@@ -1143,8 +1159,11 @@
       <c r="K6" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>1020034170</v>
       </c>
@@ -1178,8 +1197,11 @@
       <c r="K7">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>1020035180</v>
       </c>
@@ -1213,8 +1235,11 @@
       <c r="K8" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>1020040190</v>
       </c>
@@ -1248,8 +1273,11 @@
       <c r="K9" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>2020000010</v>
       </c>
@@ -1283,8 +1311,11 @@
       <c r="K10">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>2020003440</v>
       </c>
@@ -1318,8 +1349,11 @@
       <c r="K11">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>2020018240</v>
       </c>
@@ -1353,8 +1387,11 @@
       <c r="K12">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>2020024230</v>
       </c>
@@ -1388,8 +1425,11 @@
       <c r="K13">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>2020033490</v>
       </c>
@@ -1423,8 +1463,11 @@
       <c r="K14">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>2020041390</v>
       </c>
@@ -1458,8 +1501,11 @@
       <c r="K15">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>2020057170</v>
       </c>
@@ -1493,8 +1539,11 @@
       <c r="K16">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>2020065840</v>
       </c>
@@ -1528,8 +1577,11 @@
       <c r="K17">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>2020071190</v>
       </c>
@@ -1563,8 +1615,11 @@
       <c r="K18" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>3020000010</v>
       </c>
@@ -1598,8 +1653,11 @@
       <c r="K19">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>3020003790</v>
       </c>
@@ -1633,8 +1691,11 @@
       <c r="K20">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>3020005240</v>
       </c>
@@ -1668,8 +1729,11 @@
       <c r="K21">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>3020008670</v>
       </c>
@@ -1703,8 +1767,11 @@
       <c r="K22">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>3020009320</v>
       </c>
@@ -1738,8 +1805,11 @@
       <c r="K23">
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>3020024310</v>
       </c>
@@ -1773,8 +1843,11 @@
       <c r="K24" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>4020000010</v>
       </c>
@@ -1808,8 +1881,11 @@
       <c r="K25">
         <v>1</v>
       </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>4020006940</v>
       </c>
@@ -1843,8 +1919,11 @@
       <c r="K26">
         <v>1</v>
       </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>4020015090</v>
       </c>
@@ -1878,8 +1957,11 @@
       <c r="K27">
         <v>1</v>
       </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>4020024190</v>
       </c>
@@ -1913,8 +1995,11 @@
       <c r="K28">
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A29" s="2">
         <v>4020034510</v>
       </c>
@@ -1948,8 +2033,11 @@
       <c r="K29" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>4020050210</v>
       </c>
@@ -1983,8 +2071,11 @@
       <c r="K30" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>4020050220</v>
       </c>
@@ -2018,8 +2109,11 @@
       <c r="K31">
         <v>1</v>
       </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>4020050290</v>
       </c>
@@ -2053,8 +2147,11 @@
       <c r="K32" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>4020050470</v>
       </c>
@@ -2088,8 +2185,11 @@
       <c r="K33" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A34" s="2">
         <v>5020000010</v>
       </c>
@@ -2123,8 +2223,11 @@
       <c r="K34" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A35" s="2">
         <v>5020015660</v>
       </c>
@@ -2158,8 +2261,11 @@
       <c r="K35" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A36" s="2">
         <v>5020037270</v>
       </c>
@@ -2193,8 +2299,11 @@
       <c r="K36" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
         <v>5020049720</v>
       </c>
@@ -2228,8 +2337,11 @@
       <c r="K37" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>5020054880</v>
       </c>
@@ -2263,8 +2375,11 @@
       <c r="K38">
         <v>1</v>
       </c>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>5020055870</v>
       </c>
@@ -2298,8 +2413,11 @@
       <c r="K39">
         <v>1</v>
       </c>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>5020082270</v>
       </c>
@@ -2333,8 +2451,11 @@
       <c r="K40">
         <v>1</v>
       </c>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>6020000010</v>
       </c>
@@ -2368,8 +2489,11 @@
       <c r="K41">
         <v>1</v>
       </c>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>6020006540</v>
       </c>
@@ -2403,8 +2527,11 @@
       <c r="K42">
         <v>1</v>
       </c>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>6020008320</v>
       </c>
@@ -2438,8 +2565,11 @@
       <c r="K43">
         <v>1</v>
       </c>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>6020014330</v>
       </c>
@@ -2473,8 +2603,11 @@
       <c r="K44">
         <v>1</v>
       </c>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>6020017370</v>
       </c>
@@ -2508,8 +2641,11 @@
       <c r="K45">
         <v>1</v>
       </c>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>6020021870</v>
       </c>
@@ -2543,8 +2679,11 @@
       <c r="K46">
         <v>1</v>
       </c>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>6020029280</v>
       </c>
@@ -2578,8 +2717,11 @@
       <c r="K47">
         <v>1</v>
       </c>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>7020000010</v>
       </c>
@@ -2613,8 +2755,11 @@
       <c r="K48">
         <v>1</v>
       </c>
-    </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>7020014250</v>
       </c>
@@ -2648,8 +2793,11 @@
       <c r="K49">
         <v>1</v>
       </c>
-    </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
         <v>7020021430</v>
       </c>
@@ -2683,8 +2831,11 @@
       <c r="K50" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>7020024600</v>
       </c>
@@ -2718,8 +2869,11 @@
       <c r="K51">
         <v>1</v>
       </c>
-    </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>7020038340</v>
       </c>
@@ -2753,8 +2907,11 @@
       <c r="K52">
         <v>1</v>
       </c>
-    </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L52">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>7020046750</v>
       </c>
@@ -2788,8 +2945,11 @@
       <c r="K53">
         <v>1</v>
       </c>
-    </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>7020047840</v>
       </c>
@@ -2823,8 +2983,11 @@
       <c r="K54">
         <v>1</v>
       </c>
-    </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A55" s="2">
         <v>7020065090</v>
       </c>
@@ -2858,8 +3021,11 @@
       <c r="K55" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L55">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A56" s="1">
         <v>8020000010</v>
       </c>
@@ -2893,8 +3059,11 @@
       <c r="K56" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L56">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A57" s="1">
         <v>8020008900</v>
       </c>
@@ -2928,8 +3097,11 @@
       <c r="K57" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L57">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>8020010700</v>
       </c>
@@ -2963,8 +3135,11 @@
       <c r="K58">
         <v>1</v>
       </c>
-    </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L58">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>8020020760</v>
       </c>
@@ -2998,8 +3173,11 @@
       <c r="K59">
         <v>1</v>
       </c>
-    </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>8020022890</v>
       </c>
@@ -3033,8 +3211,11 @@
       <c r="K60">
         <v>1</v>
       </c>
-    </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L60">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>8020032840</v>
       </c>
@@ -3068,8 +3249,11 @@
       <c r="K61">
         <v>1</v>
       </c>
-    </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L61">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>8020044560</v>
       </c>
@@ -3103,8 +3287,11 @@
       <c r="K62">
         <v>1</v>
       </c>
-    </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L62">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>9020000010</v>
       </c>
@@ -3136,6 +3323,9 @@
         <v>1</v>
       </c>
       <c r="K63">
+        <v>1</v>
+      </c>
+      <c r="L63">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
full lake, island, and low flow removal - increased performance
</commit_message>
<xml_diff>
--- a/tdxhydrorapid/network_data/processing_options.xlsx
+++ b/tdxhydrorapid/network_data/processing_options.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ricky/tdxhydro-postprocessing/tdxhydrorapid/network_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23A23C73-A551-C147-82F6-B1ECE8D77723}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA3E714F-879F-D147-9E0A-E109EA50BC8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="500" windowWidth="34560" windowHeight="20120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2160" yWindow="3840" windowWidth="45500" windowHeight="20120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="region_label_numbers" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>min_stream_order</t>
   </si>
@@ -59,6 +59,18 @@
   </si>
   <si>
     <t>dissolve_lakes</t>
+  </si>
+  <si>
+    <t>drop_islands</t>
+  </si>
+  <si>
+    <t>drop_ocean_watersheds</t>
+  </si>
+  <si>
+    <t>drop_within_sea</t>
+  </si>
+  <si>
+    <t>drop_low_flow</t>
   </si>
 </sst>
 </file>
@@ -913,11 +925,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L63"/>
+  <dimension ref="A1:P63"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N57" sqref="N57"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="Q2" sqref="Q2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -925,7 +937,7 @@
     <col min="1" max="1" width="13.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.83203125" customWidth="1"/>
     <col min="3" max="3" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.83203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18.5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16.83203125" bestFit="1" customWidth="1"/>
@@ -933,9 +945,14 @@
     <col min="9" max="9" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="17.1640625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -972,8 +989,20 @@
       <c r="L1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1020000010</v>
       </c>
@@ -1010,8 +1039,20 @@
       <c r="L2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M2">
+        <v>1</v>
+      </c>
+      <c r="N2">
+        <v>1</v>
+      </c>
+      <c r="O2">
+        <v>1</v>
+      </c>
+      <c r="P2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1020011530</v>
       </c>
@@ -1048,8 +1089,20 @@
       <c r="L3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M3">
+        <v>1</v>
+      </c>
+      <c r="N3">
+        <v>1</v>
+      </c>
+      <c r="O3">
+        <v>1</v>
+      </c>
+      <c r="P3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1020018110</v>
       </c>
@@ -1086,8 +1139,20 @@
       <c r="L4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M4">
+        <v>1</v>
+      </c>
+      <c r="N4">
+        <v>1</v>
+      </c>
+      <c r="O4">
+        <v>1</v>
+      </c>
+      <c r="P4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1020021940</v>
       </c>
@@ -1124,8 +1189,20 @@
       <c r="L5">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M5">
+        <v>1</v>
+      </c>
+      <c r="N5">
+        <v>1</v>
+      </c>
+      <c r="O5">
+        <v>1</v>
+      </c>
+      <c r="P5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>1020027430</v>
       </c>
@@ -1162,8 +1239,20 @@
       <c r="L6">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M6">
+        <v>1</v>
+      </c>
+      <c r="N6">
+        <v>1</v>
+      </c>
+      <c r="O6">
+        <v>1</v>
+      </c>
+      <c r="P6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>1020034170</v>
       </c>
@@ -1200,8 +1289,20 @@
       <c r="L7">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M7">
+        <v>1</v>
+      </c>
+      <c r="N7">
+        <v>1</v>
+      </c>
+      <c r="O7">
+        <v>1</v>
+      </c>
+      <c r="P7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>1020035180</v>
       </c>
@@ -1238,8 +1339,20 @@
       <c r="L8">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M8">
+        <v>1</v>
+      </c>
+      <c r="N8">
+        <v>1</v>
+      </c>
+      <c r="O8">
+        <v>1</v>
+      </c>
+      <c r="P8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>1020040190</v>
       </c>
@@ -1276,8 +1389,20 @@
       <c r="L9">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M9">
+        <v>1</v>
+      </c>
+      <c r="N9">
+        <v>1</v>
+      </c>
+      <c r="O9">
+        <v>1</v>
+      </c>
+      <c r="P9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>2020000010</v>
       </c>
@@ -1314,8 +1439,20 @@
       <c r="L10">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M10">
+        <v>1</v>
+      </c>
+      <c r="N10">
+        <v>1</v>
+      </c>
+      <c r="O10">
+        <v>1</v>
+      </c>
+      <c r="P10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>2020003440</v>
       </c>
@@ -1352,8 +1489,20 @@
       <c r="L11">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M11">
+        <v>1</v>
+      </c>
+      <c r="N11">
+        <v>1</v>
+      </c>
+      <c r="O11">
+        <v>1</v>
+      </c>
+      <c r="P11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>2020018240</v>
       </c>
@@ -1390,8 +1539,20 @@
       <c r="L12">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M12">
+        <v>1</v>
+      </c>
+      <c r="N12">
+        <v>1</v>
+      </c>
+      <c r="O12">
+        <v>1</v>
+      </c>
+      <c r="P12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>2020024230</v>
       </c>
@@ -1428,8 +1589,20 @@
       <c r="L13">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M13">
+        <v>1</v>
+      </c>
+      <c r="N13">
+        <v>1</v>
+      </c>
+      <c r="O13">
+        <v>1</v>
+      </c>
+      <c r="P13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>2020033490</v>
       </c>
@@ -1466,8 +1639,20 @@
       <c r="L14">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M14">
+        <v>1</v>
+      </c>
+      <c r="N14">
+        <v>1</v>
+      </c>
+      <c r="O14">
+        <v>1</v>
+      </c>
+      <c r="P14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>2020041390</v>
       </c>
@@ -1504,8 +1689,20 @@
       <c r="L15">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M15">
+        <v>1</v>
+      </c>
+      <c r="N15">
+        <v>1</v>
+      </c>
+      <c r="O15">
+        <v>1</v>
+      </c>
+      <c r="P15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>2020057170</v>
       </c>
@@ -1542,8 +1739,20 @@
       <c r="L16">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M16">
+        <v>1</v>
+      </c>
+      <c r="N16">
+        <v>1</v>
+      </c>
+      <c r="O16">
+        <v>1</v>
+      </c>
+      <c r="P16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>2020065840</v>
       </c>
@@ -1580,8 +1789,20 @@
       <c r="L17">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M17">
+        <v>1</v>
+      </c>
+      <c r="N17">
+        <v>1</v>
+      </c>
+      <c r="O17">
+        <v>1</v>
+      </c>
+      <c r="P17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>2020071190</v>
       </c>
@@ -1618,8 +1839,20 @@
       <c r="L18">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M18">
+        <v>1</v>
+      </c>
+      <c r="N18">
+        <v>1</v>
+      </c>
+      <c r="O18">
+        <v>1</v>
+      </c>
+      <c r="P18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>3020000010</v>
       </c>
@@ -1656,8 +1889,20 @@
       <c r="L19">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M19">
+        <v>1</v>
+      </c>
+      <c r="N19">
+        <v>1</v>
+      </c>
+      <c r="O19">
+        <v>1</v>
+      </c>
+      <c r="P19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>3020003790</v>
       </c>
@@ -1694,8 +1939,20 @@
       <c r="L20">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M20">
+        <v>1</v>
+      </c>
+      <c r="N20">
+        <v>1</v>
+      </c>
+      <c r="O20">
+        <v>1</v>
+      </c>
+      <c r="P20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>3020005240</v>
       </c>
@@ -1732,8 +1989,20 @@
       <c r="L21">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M21">
+        <v>1</v>
+      </c>
+      <c r="N21">
+        <v>1</v>
+      </c>
+      <c r="O21">
+        <v>1</v>
+      </c>
+      <c r="P21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>3020008670</v>
       </c>
@@ -1770,8 +2039,20 @@
       <c r="L22">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M22">
+        <v>1</v>
+      </c>
+      <c r="N22">
+        <v>1</v>
+      </c>
+      <c r="O22">
+        <v>1</v>
+      </c>
+      <c r="P22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>3020009320</v>
       </c>
@@ -1808,8 +2089,20 @@
       <c r="L23">
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M23">
+        <v>1</v>
+      </c>
+      <c r="N23">
+        <v>1</v>
+      </c>
+      <c r="O23">
+        <v>1</v>
+      </c>
+      <c r="P23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>3020024310</v>
       </c>
@@ -1846,8 +2139,20 @@
       <c r="L24">
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M24">
+        <v>1</v>
+      </c>
+      <c r="N24">
+        <v>1</v>
+      </c>
+      <c r="O24">
+        <v>1</v>
+      </c>
+      <c r="P24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>4020000010</v>
       </c>
@@ -1884,8 +2189,20 @@
       <c r="L25">
         <v>1</v>
       </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M25">
+        <v>1</v>
+      </c>
+      <c r="N25">
+        <v>1</v>
+      </c>
+      <c r="O25">
+        <v>1</v>
+      </c>
+      <c r="P25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>4020006940</v>
       </c>
@@ -1922,8 +2239,20 @@
       <c r="L26">
         <v>1</v>
       </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M26">
+        <v>1</v>
+      </c>
+      <c r="N26">
+        <v>1</v>
+      </c>
+      <c r="O26">
+        <v>1</v>
+      </c>
+      <c r="P26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>4020015090</v>
       </c>
@@ -1960,8 +2289,20 @@
       <c r="L27">
         <v>1</v>
       </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M27">
+        <v>1</v>
+      </c>
+      <c r="N27">
+        <v>1</v>
+      </c>
+      <c r="O27">
+        <v>1</v>
+      </c>
+      <c r="P27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>4020024190</v>
       </c>
@@ -1998,8 +2339,20 @@
       <c r="L28">
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M28">
+        <v>1</v>
+      </c>
+      <c r="N28">
+        <v>1</v>
+      </c>
+      <c r="O28">
+        <v>1</v>
+      </c>
+      <c r="P28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A29" s="2">
         <v>4020034510</v>
       </c>
@@ -2036,8 +2389,20 @@
       <c r="L29">
         <v>1</v>
       </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M29">
+        <v>1</v>
+      </c>
+      <c r="N29">
+        <v>1</v>
+      </c>
+      <c r="O29">
+        <v>1</v>
+      </c>
+      <c r="P29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>4020050210</v>
       </c>
@@ -2074,8 +2439,20 @@
       <c r="L30">
         <v>1</v>
       </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M30">
+        <v>1</v>
+      </c>
+      <c r="N30">
+        <v>1</v>
+      </c>
+      <c r="O30">
+        <v>1</v>
+      </c>
+      <c r="P30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>4020050220</v>
       </c>
@@ -2112,8 +2489,20 @@
       <c r="L31">
         <v>1</v>
       </c>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M31">
+        <v>1</v>
+      </c>
+      <c r="N31">
+        <v>1</v>
+      </c>
+      <c r="O31">
+        <v>1</v>
+      </c>
+      <c r="P31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>4020050290</v>
       </c>
@@ -2150,8 +2539,20 @@
       <c r="L32">
         <v>1</v>
       </c>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M32">
+        <v>1</v>
+      </c>
+      <c r="N32">
+        <v>1</v>
+      </c>
+      <c r="O32">
+        <v>1</v>
+      </c>
+      <c r="P32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>4020050470</v>
       </c>
@@ -2188,8 +2589,20 @@
       <c r="L33">
         <v>1</v>
       </c>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M33">
+        <v>1</v>
+      </c>
+      <c r="N33">
+        <v>1</v>
+      </c>
+      <c r="O33">
+        <v>1</v>
+      </c>
+      <c r="P33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A34" s="2">
         <v>5020000010</v>
       </c>
@@ -2226,8 +2639,20 @@
       <c r="L34">
         <v>1</v>
       </c>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M34">
+        <v>1</v>
+      </c>
+      <c r="N34">
+        <v>1</v>
+      </c>
+      <c r="O34">
+        <v>1</v>
+      </c>
+      <c r="P34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A35" s="2">
         <v>5020015660</v>
       </c>
@@ -2264,8 +2689,20 @@
       <c r="L35">
         <v>1</v>
       </c>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M35">
+        <v>1</v>
+      </c>
+      <c r="N35">
+        <v>1</v>
+      </c>
+      <c r="O35">
+        <v>1</v>
+      </c>
+      <c r="P35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A36" s="2">
         <v>5020037270</v>
       </c>
@@ -2302,8 +2739,20 @@
       <c r="L36">
         <v>1</v>
       </c>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M36">
+        <v>1</v>
+      </c>
+      <c r="N36">
+        <v>1</v>
+      </c>
+      <c r="O36">
+        <v>1</v>
+      </c>
+      <c r="P36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
         <v>5020049720</v>
       </c>
@@ -2340,8 +2789,20 @@
       <c r="L37">
         <v>1</v>
       </c>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M37">
+        <v>1</v>
+      </c>
+      <c r="N37">
+        <v>1</v>
+      </c>
+      <c r="O37">
+        <v>1</v>
+      </c>
+      <c r="P37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>5020054880</v>
       </c>
@@ -2378,8 +2839,20 @@
       <c r="L38">
         <v>1</v>
       </c>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M38">
+        <v>1</v>
+      </c>
+      <c r="N38">
+        <v>1</v>
+      </c>
+      <c r="O38">
+        <v>1</v>
+      </c>
+      <c r="P38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>5020055870</v>
       </c>
@@ -2416,8 +2889,20 @@
       <c r="L39">
         <v>1</v>
       </c>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M39">
+        <v>1</v>
+      </c>
+      <c r="N39">
+        <v>1</v>
+      </c>
+      <c r="O39">
+        <v>1</v>
+      </c>
+      <c r="P39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>5020082270</v>
       </c>
@@ -2454,8 +2939,20 @@
       <c r="L40">
         <v>1</v>
       </c>
-    </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M40">
+        <v>1</v>
+      </c>
+      <c r="N40">
+        <v>1</v>
+      </c>
+      <c r="O40">
+        <v>1</v>
+      </c>
+      <c r="P40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>6020000010</v>
       </c>
@@ -2492,8 +2989,20 @@
       <c r="L41">
         <v>1</v>
       </c>
-    </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M41">
+        <v>1</v>
+      </c>
+      <c r="N41">
+        <v>1</v>
+      </c>
+      <c r="O41">
+        <v>1</v>
+      </c>
+      <c r="P41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>6020006540</v>
       </c>
@@ -2530,8 +3039,20 @@
       <c r="L42">
         <v>1</v>
       </c>
-    </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M42">
+        <v>1</v>
+      </c>
+      <c r="N42">
+        <v>1</v>
+      </c>
+      <c r="O42">
+        <v>1</v>
+      </c>
+      <c r="P42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>6020008320</v>
       </c>
@@ -2568,8 +3089,20 @@
       <c r="L43">
         <v>1</v>
       </c>
-    </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M43">
+        <v>1</v>
+      </c>
+      <c r="N43">
+        <v>1</v>
+      </c>
+      <c r="O43">
+        <v>1</v>
+      </c>
+      <c r="P43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>6020014330</v>
       </c>
@@ -2606,8 +3139,20 @@
       <c r="L44">
         <v>1</v>
       </c>
-    </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M44">
+        <v>1</v>
+      </c>
+      <c r="N44">
+        <v>1</v>
+      </c>
+      <c r="O44">
+        <v>1</v>
+      </c>
+      <c r="P44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>6020017370</v>
       </c>
@@ -2644,8 +3189,20 @@
       <c r="L45">
         <v>1</v>
       </c>
-    </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M45">
+        <v>1</v>
+      </c>
+      <c r="N45">
+        <v>1</v>
+      </c>
+      <c r="O45">
+        <v>1</v>
+      </c>
+      <c r="P45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>6020021870</v>
       </c>
@@ -2682,8 +3239,20 @@
       <c r="L46">
         <v>1</v>
       </c>
-    </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M46">
+        <v>1</v>
+      </c>
+      <c r="N46">
+        <v>1</v>
+      </c>
+      <c r="O46">
+        <v>1</v>
+      </c>
+      <c r="P46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>6020029280</v>
       </c>
@@ -2720,8 +3289,20 @@
       <c r="L47">
         <v>1</v>
       </c>
-    </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M47">
+        <v>1</v>
+      </c>
+      <c r="N47">
+        <v>1</v>
+      </c>
+      <c r="O47">
+        <v>1</v>
+      </c>
+      <c r="P47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>7020000010</v>
       </c>
@@ -2758,8 +3339,20 @@
       <c r="L48">
         <v>1</v>
       </c>
-    </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M48">
+        <v>1</v>
+      </c>
+      <c r="N48">
+        <v>1</v>
+      </c>
+      <c r="O48">
+        <v>1</v>
+      </c>
+      <c r="P48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>7020014250</v>
       </c>
@@ -2796,8 +3389,20 @@
       <c r="L49">
         <v>1</v>
       </c>
-    </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M49">
+        <v>1</v>
+      </c>
+      <c r="N49">
+        <v>1</v>
+      </c>
+      <c r="O49">
+        <v>1</v>
+      </c>
+      <c r="P49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
         <v>7020021430</v>
       </c>
@@ -2834,8 +3439,20 @@
       <c r="L50">
         <v>1</v>
       </c>
-    </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M50">
+        <v>1</v>
+      </c>
+      <c r="N50">
+        <v>1</v>
+      </c>
+      <c r="O50">
+        <v>1</v>
+      </c>
+      <c r="P50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>7020024600</v>
       </c>
@@ -2872,8 +3489,20 @@
       <c r="L51">
         <v>1</v>
       </c>
-    </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M51">
+        <v>1</v>
+      </c>
+      <c r="N51">
+        <v>1</v>
+      </c>
+      <c r="O51">
+        <v>1</v>
+      </c>
+      <c r="P51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>7020038340</v>
       </c>
@@ -2910,8 +3539,20 @@
       <c r="L52">
         <v>1</v>
       </c>
-    </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M52">
+        <v>1</v>
+      </c>
+      <c r="N52">
+        <v>1</v>
+      </c>
+      <c r="O52">
+        <v>1</v>
+      </c>
+      <c r="P52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>7020046750</v>
       </c>
@@ -2948,8 +3589,20 @@
       <c r="L53">
         <v>1</v>
       </c>
-    </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M53">
+        <v>1</v>
+      </c>
+      <c r="N53">
+        <v>1</v>
+      </c>
+      <c r="O53">
+        <v>1</v>
+      </c>
+      <c r="P53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>7020047840</v>
       </c>
@@ -2986,8 +3639,20 @@
       <c r="L54">
         <v>1</v>
       </c>
-    </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M54">
+        <v>1</v>
+      </c>
+      <c r="N54">
+        <v>1</v>
+      </c>
+      <c r="O54">
+        <v>1</v>
+      </c>
+      <c r="P54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A55" s="2">
         <v>7020065090</v>
       </c>
@@ -3024,8 +3689,20 @@
       <c r="L55">
         <v>1</v>
       </c>
-    </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M55">
+        <v>1</v>
+      </c>
+      <c r="N55">
+        <v>1</v>
+      </c>
+      <c r="O55">
+        <v>1</v>
+      </c>
+      <c r="P55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A56" s="1">
         <v>8020000010</v>
       </c>
@@ -3062,8 +3739,20 @@
       <c r="L56">
         <v>1</v>
       </c>
-    </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M56">
+        <v>1</v>
+      </c>
+      <c r="N56">
+        <v>1</v>
+      </c>
+      <c r="O56">
+        <v>1</v>
+      </c>
+      <c r="P56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A57" s="1">
         <v>8020008900</v>
       </c>
@@ -3100,8 +3789,20 @@
       <c r="L57">
         <v>1</v>
       </c>
-    </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M57">
+        <v>1</v>
+      </c>
+      <c r="N57">
+        <v>1</v>
+      </c>
+      <c r="O57">
+        <v>1</v>
+      </c>
+      <c r="P57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>8020010700</v>
       </c>
@@ -3138,8 +3839,20 @@
       <c r="L58">
         <v>1</v>
       </c>
-    </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M58">
+        <v>1</v>
+      </c>
+      <c r="N58">
+        <v>1</v>
+      </c>
+      <c r="O58">
+        <v>1</v>
+      </c>
+      <c r="P58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>8020020760</v>
       </c>
@@ -3176,8 +3889,20 @@
       <c r="L59">
         <v>1</v>
       </c>
-    </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M59">
+        <v>1</v>
+      </c>
+      <c r="N59">
+        <v>1</v>
+      </c>
+      <c r="O59">
+        <v>1</v>
+      </c>
+      <c r="P59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>8020022890</v>
       </c>
@@ -3214,8 +3939,20 @@
       <c r="L60">
         <v>1</v>
       </c>
-    </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M60">
+        <v>1</v>
+      </c>
+      <c r="N60">
+        <v>1</v>
+      </c>
+      <c r="O60">
+        <v>1</v>
+      </c>
+      <c r="P60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>8020032840</v>
       </c>
@@ -3252,8 +3989,20 @@
       <c r="L61">
         <v>1</v>
       </c>
-    </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M61">
+        <v>1</v>
+      </c>
+      <c r="N61">
+        <v>1</v>
+      </c>
+      <c r="O61">
+        <v>1</v>
+      </c>
+      <c r="P61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>8020044560</v>
       </c>
@@ -3290,8 +4039,20 @@
       <c r="L62">
         <v>1</v>
       </c>
-    </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M62">
+        <v>1</v>
+      </c>
+      <c r="N62">
+        <v>1</v>
+      </c>
+      <c r="O62">
+        <v>1</v>
+      </c>
+      <c r="P62">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>9020000010</v>
       </c>
@@ -3327,6 +4088,18 @@
       </c>
       <c r="L63">
         <v>1</v>
+      </c>
+      <c r="M63">
+        <v>1</v>
+      </c>
+      <c r="N63">
+        <v>1</v>
+      </c>
+      <c r="O63">
+        <v>1</v>
+      </c>
+      <c r="P63">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>